<commit_message>
config and test 6-16-2021
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Timings</t>
   </si>
@@ -28,18 +28,6 @@
   </si>
   <si>
     <t>Passcode</t>
-  </si>
-  <si>
-    <t>925 7400 2970</t>
-  </si>
-  <si>
-    <t>GE7ce7</t>
-  </si>
-  <si>
-    <t>225 7430 3970</t>
-  </si>
-  <si>
-    <t>Df3daf</t>
   </si>
 </sst>
 </file>
@@ -371,13 +359,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,27 +376,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="B2">
+        <v>3442836988</v>
+      </c>
+      <c r="C2">
+        <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.67222222222222217</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>